<commit_message>
created several train/test sets. several models and training metrics and results too
</commit_message>
<xml_diff>
--- a/models/training_metrics.xlsx
+++ b/models/training_metrics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\01eco\Documents\Programming\Python\multisource_ML_research\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3940E250-ADF1-4815-869E-94A1AAC9F29F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10CB33FC-EF1F-4E7A-8C0A-C40FA75A1982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="771" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="25">
   <si>
     <t>SVM</t>
   </si>
@@ -111,16 +111,10 @@
     <t>MLP</t>
   </si>
   <si>
-    <t>Sum</t>
+    <t>SVM (C=10,kernel='rbf',gamma=0.1)</t>
   </si>
   <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
+    <t>Is_Gaze_on_Hazard</t>
   </si>
 </sst>
 </file>
@@ -177,11 +171,29 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -192,7 +204,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -205,6 +217,36 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Accent2" xfId="2" builtinId="34"/>
@@ -1383,6 +1425,94 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>139</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>162</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A8ADD11-1256-8ABE-6842-796F1ACFDCC1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2400300" y="26479500"/>
+          <a:ext cx="5391150" cy="4467225"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>163</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>186</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E967FEDB-BE0B-C6EA-F210-DC8C3D5D7351}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2400300" y="31051500"/>
+          <a:ext cx="5391150" cy="4467225"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1649,1327 +1779,1626 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9050775-3EE0-4444-BC69-86A15CAD3B8E}">
-  <dimension ref="A1:Y13"/>
+  <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G22" sqref="G22"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="25" width="15.7109375" customWidth="1"/>
+    <col min="1" max="27" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="4" t="str">
+      <c r="B1" s="7" t="str">
         <f>window_size_20!B1</f>
         <v>SVM</v>
       </c>
-      <c r="C1" s="4" t="str">
+      <c r="C1" s="7" t="str">
         <f>window_size_20!B25</f>
         <v>SVM</v>
       </c>
-      <c r="D1" s="3" t="str">
+      <c r="D1" s="8" t="str">
         <f>window_size_20!B48</f>
         <v>SVM</v>
       </c>
-      <c r="E1" s="3" t="str">
+      <c r="E1" s="8" t="str">
         <f>window_size_20!B71</f>
         <v>SVM</v>
       </c>
-      <c r="F1" s="3" t="str">
+      <c r="F1" s="8" t="str">
         <f>window_size_20!B94</f>
         <v>RF</v>
       </c>
-      <c r="G1" s="3" t="str">
+      <c r="G1" s="8" t="str">
         <f>window_size_20!B117</f>
         <v>MLP</v>
       </c>
-      <c r="H1" s="4" t="str">
+      <c r="H1" s="9" t="str">
+        <f>window_size_20!B140</f>
+        <v>SVM (C=10,kernel='rbf',gamma=0.1)</v>
+      </c>
+      <c r="I1" s="9" t="str">
+        <f>window_size_20!B164</f>
+        <v>SVM (C=10,kernel='rbf',gamma=0.1)</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="7">
+        <f>window_size_20!B2</f>
+        <v>20</v>
+      </c>
+      <c r="C2" s="7">
+        <f>window_size_20!B26</f>
+        <v>20</v>
+      </c>
+      <c r="D2" s="8">
+        <f>window_size_20!B49</f>
+        <v>20</v>
+      </c>
+      <c r="E2" s="8">
+        <f>window_size_20!B72</f>
+        <v>20</v>
+      </c>
+      <c r="F2" s="8">
+        <f>window_size_20!B95</f>
+        <v>20</v>
+      </c>
+      <c r="G2" s="8">
+        <f>window_size_20!B118</f>
+        <v>20</v>
+      </c>
+      <c r="H2" s="9">
+        <f>window_size_20!B141</f>
+        <v>20</v>
+      </c>
+      <c r="I2" s="9">
+        <f>window_size_20!B165</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7" t="str">
+        <f>window_size_20!B3</f>
+        <v>No</v>
+      </c>
+      <c r="C3" s="7" t="str">
+        <f>window_size_20!B27</f>
+        <v>No</v>
+      </c>
+      <c r="D3" s="8" t="str">
+        <f>window_size_20!B50</f>
+        <v>Yes</v>
+      </c>
+      <c r="E3" s="8" t="str">
+        <f>window_size_20!B73</f>
+        <v>Yes</v>
+      </c>
+      <c r="F3" s="8" t="str">
+        <f>window_size_20!B96</f>
+        <v>Yes</v>
+      </c>
+      <c r="G3" s="8" t="str">
+        <f>window_size_20!B119</f>
+        <v>Yes</v>
+      </c>
+      <c r="H3" s="9" t="str">
+        <f>window_size_20!B142</f>
+        <v>Yes</v>
+      </c>
+      <c r="I3" s="9" t="str">
+        <f>window_size_20!B166</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="7" t="str">
+        <f>window_size_20!B4</f>
+        <v>All</v>
+      </c>
+      <c r="C4" s="7" t="str">
+        <f>window_size_20!B28</f>
+        <v>Is_Gaze_On_Hazard</v>
+      </c>
+      <c r="D4" s="8" t="str">
+        <f>window_size_20!B51</f>
+        <v>Is_Gaze_On_Hazard</v>
+      </c>
+      <c r="E4" s="8" t="str">
+        <f>window_size_20!B74</f>
+        <v>Is_Gaze_On_Hazard</v>
+      </c>
+      <c r="F4" s="8" t="str">
+        <f>window_size_20!B97</f>
+        <v>Is_Gaze_On_Hazard</v>
+      </c>
+      <c r="G4" s="8" t="str">
+        <f>window_size_20!B120</f>
+        <v>Is_Gaze_On_Hazard</v>
+      </c>
+      <c r="H4" s="9" t="str">
+        <f>window_size_20!B143</f>
+        <v>Is_Gaze_on_Hazard</v>
+      </c>
+      <c r="I4" s="9" t="str">
+        <f>window_size_20!B167</f>
+        <v>Is_Gaze_on_Hazard</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="7">
+        <f>window_size_20!B5</f>
+        <v>31023</v>
+      </c>
+      <c r="C5" s="7">
+        <f>window_size_20!B29</f>
+        <v>31023</v>
+      </c>
+      <c r="D5" s="8">
+        <f>window_size_20!B52</f>
+        <v>31023</v>
+      </c>
+      <c r="E5" s="8">
+        <f>window_size_20!B75</f>
+        <v>59512</v>
+      </c>
+      <c r="F5" s="8">
+        <f>window_size_20!B98</f>
+        <v>31023</v>
+      </c>
+      <c r="G5" s="8">
+        <f>window_size_20!B121</f>
+        <v>31023</v>
+      </c>
+      <c r="H5" s="9">
+        <f>window_size_20!B144</f>
+        <v>31023</v>
+      </c>
+      <c r="I5" s="9">
+        <f>window_size_20!B168</f>
+        <v>59512</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="7">
+        <f>window_size_20!B6</f>
+        <v>0</v>
+      </c>
+      <c r="C6" s="7">
+        <f>window_size_20!B30</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="8">
+        <f>window_size_20!B53</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="8">
+        <f>window_size_20!B76</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="8">
+        <f>window_size_20!B99</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="8">
+        <f>window_size_20!B122</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="9">
+        <f>window_size_20!B145</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="9">
+        <f>window_size_20!B169</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="7" t="str">
+        <f>window_size_20!B7</f>
+        <v>NAN</v>
+      </c>
+      <c r="C7" s="7">
+        <f>window_size_20!B31</f>
+        <v>0.50731707317073105</v>
+      </c>
+      <c r="D7" s="8">
+        <f>window_size_20!B54</f>
+        <v>0.206561360874848</v>
+      </c>
+      <c r="E7" s="8">
+        <f>window_size_20!B77</f>
+        <v>0.231634885901844</v>
+      </c>
+      <c r="F7" s="8">
+        <f>window_size_20!B100</f>
+        <v>0.19160387513455299</v>
+      </c>
+      <c r="G7" s="8">
+        <f>window_size_20!B123</f>
+        <v>0.223188405797101</v>
+      </c>
+      <c r="H7" s="9">
+        <f>window_size_20!B146</f>
+        <v>0.21118012422360199</v>
+      </c>
+      <c r="I7" s="9">
+        <f>window_size_20!B170</f>
+        <v>0.23651452282157601</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="7">
+        <f>window_size_20!B8</f>
+        <v>0</v>
+      </c>
+      <c r="C8" s="7">
+        <f>window_size_20!B32</f>
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="D8" s="8">
+        <f>window_size_20!B55</f>
+        <v>0.104615384615384</v>
+      </c>
+      <c r="E8" s="8">
+        <f>window_size_20!B78</f>
+        <v>1</v>
+      </c>
+      <c r="F8" s="8">
+        <f>window_size_20!B101</f>
+        <v>0.109538461538461</v>
+      </c>
+      <c r="G8" s="8">
+        <f>window_size_20!B124</f>
+        <v>9.4769230769230703E-2</v>
+      </c>
+      <c r="H8" s="9">
+        <f>window_size_20!B147</f>
+        <v>0.104615384615384</v>
+      </c>
+      <c r="I8" s="9">
+        <f>window_size_20!B171</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="7" t="str">
+        <f>window_size_20!B9</f>
+        <v>NAN</v>
+      </c>
+      <c r="C9" s="7">
+        <f>window_size_20!B33</f>
+        <v>0.113661202185792</v>
+      </c>
+      <c r="D9" s="8">
+        <f>window_size_20!B56</f>
+        <v>0.13888888888888801</v>
+      </c>
+      <c r="E9" s="8">
+        <f>window_size_20!B79</f>
+        <v>0.37614213197969498</v>
+      </c>
+      <c r="F9" s="8">
+        <f>window_size_20!B102</f>
+        <v>0.139389193422083</v>
+      </c>
+      <c r="G9" s="8">
+        <f>window_size_20!B125</f>
+        <v>0.13304535637149001</v>
+      </c>
+      <c r="H9" s="9">
+        <f>window_size_20!B148</f>
+        <v>0.139917695473251</v>
+      </c>
+      <c r="I9" s="9">
+        <f>window_size_20!B172</f>
+        <v>0.38255033557046902</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="7">
+        <f>window_size_20!B10</f>
+        <v>0.947619508106888</v>
+      </c>
+      <c r="C10" s="7">
+        <f>window_size_20!B34</f>
+        <v>0.94771621055346</v>
+      </c>
+      <c r="D10" s="8">
+        <f>window_size_20!B57</f>
+        <v>0.93205041420881196</v>
+      </c>
+      <c r="E10" s="8">
+        <f>window_size_20!B80</f>
+        <v>0.95869740556526395</v>
+      </c>
+      <c r="F10" s="8">
+        <f>window_size_20!B103</f>
+        <v>0.92914934081165501</v>
+      </c>
+      <c r="G10" s="8">
+        <f>window_size_20!B126</f>
+        <v>0.93530606324340004</v>
+      </c>
+      <c r="H10" s="9">
+        <f>window_size_20!B149</f>
+        <v>0.932630628888244</v>
+      </c>
+      <c r="I10" s="9">
+        <f>window_size_20!B173</f>
+        <v>0.95980642559483798</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="7">
+        <f>window_size_20!B11</f>
+        <v>1</v>
+      </c>
+      <c r="C11" s="7">
+        <f>window_size_20!B35</f>
+        <v>0.99656439213551895</v>
+      </c>
+      <c r="D11" s="8">
+        <f>window_size_20!B58</f>
+        <v>0.97778760459895198</v>
+      </c>
+      <c r="E11" s="8">
+        <f>window_size_20!B81</f>
+        <v>0.95817665175001199</v>
+      </c>
+      <c r="F11" s="8">
+        <f>window_size_20!B104</f>
+        <v>0.97445404449282202</v>
+      </c>
+      <c r="G11" s="8">
+        <f>window_size_20!B127</f>
+        <v>0.98176746717463703</v>
+      </c>
+      <c r="H11" s="9">
+        <f>window_size_20!B150</f>
+        <v>0.97839989114905701</v>
+      </c>
+      <c r="I11" s="9">
+        <f>window_size_20!B174</f>
+        <v>0.95929965459154998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="7">
+        <f>window_size_20!B12</f>
+        <v>0.5</v>
+      </c>
+      <c r="C12" s="7">
+        <f>window_size_20!B36</f>
+        <v>0.53028219606775895</v>
+      </c>
+      <c r="D12" s="8">
+        <f>window_size_20!B59</f>
+        <v>0.54120149460716804</v>
+      </c>
+      <c r="E12" s="8">
+        <f>window_size_20!B82</f>
+        <v>0.97908832587500605</v>
+      </c>
+      <c r="F12" s="8">
+        <f>window_size_20!B105</f>
+        <v>0.54199625301564203</v>
+      </c>
+      <c r="G12" s="8">
+        <f>window_size_20!B128</f>
+        <v>0.53826834897193399</v>
+      </c>
+      <c r="H12" s="9">
+        <f>window_size_20!B151</f>
+        <v>0.541507637882221</v>
+      </c>
+      <c r="I12" s="9">
+        <f>window_size_20!B175</f>
+        <v>0.97964982729577499</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="15" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="12" t="str">
+        <f>window_size_20!B13</f>
+        <v>Test</v>
+      </c>
+      <c r="C13" s="12" t="str">
+        <f>window_size_20!B37</f>
+        <v>Test</v>
+      </c>
+      <c r="D13" s="13" t="str">
+        <f>window_size_20!B60</f>
+        <v>Test</v>
+      </c>
+      <c r="E13" s="13" t="str">
+        <f>window_size_20!B83</f>
+        <v>Validation</v>
+      </c>
+      <c r="F13" s="13" t="str">
+        <f>window_size_20!B106</f>
+        <v>Test</v>
+      </c>
+      <c r="G13" s="13" t="str">
+        <f>window_size_20!B129</f>
+        <v>Test</v>
+      </c>
+      <c r="H13" s="14" t="str">
+        <f>window_size_20!B152</f>
+        <v>Test</v>
+      </c>
+      <c r="I13" s="14" t="str">
+        <f>window_size_20!B176</f>
+        <v>Validation</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="10" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="7" t="str">
         <f>window_size_15!B1</f>
         <v>SVM</v>
       </c>
-      <c r="I1" s="4" t="str">
+      <c r="C14" s="7" t="str">
         <f>window_size_15!B25</f>
         <v>SVM</v>
       </c>
-      <c r="J1" s="3" t="str">
+      <c r="D14" s="8" t="str">
         <f>window_size_15!B48</f>
         <v>SVM</v>
       </c>
-      <c r="K1" s="3" t="str">
+      <c r="E14" s="8" t="str">
         <f>window_size_15!B71</f>
         <v>SVM</v>
       </c>
-      <c r="L1" s="3" t="str">
+      <c r="F14" s="8" t="str">
         <f>window_size_15!B94</f>
         <v>RF</v>
       </c>
-      <c r="M1" s="3" t="str">
+      <c r="G14" s="8" t="str">
         <f>window_size_15!B117</f>
         <v>MLP</v>
       </c>
-      <c r="N1" s="4" t="str">
+    </row>
+    <row r="15" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="7">
+        <f>window_size_15!B2</f>
+        <v>15</v>
+      </c>
+      <c r="C15" s="7">
+        <f>window_size_15!B26</f>
+        <v>15</v>
+      </c>
+      <c r="D15" s="8">
+        <f>window_size_15!B49</f>
+        <v>15</v>
+      </c>
+      <c r="E15" s="8">
+        <f>window_size_15!B72</f>
+        <v>15</v>
+      </c>
+      <c r="F15" s="8">
+        <f>window_size_15!B95</f>
+        <v>15</v>
+      </c>
+      <c r="G15" s="8">
+        <f>window_size_15!B118</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="7" t="str">
+        <f>window_size_15!B3</f>
+        <v>No</v>
+      </c>
+      <c r="C16" s="7" t="str">
+        <f>window_size_15!B27</f>
+        <v>No</v>
+      </c>
+      <c r="D16" s="8" t="str">
+        <f>window_size_15!B50</f>
+        <v>Yes</v>
+      </c>
+      <c r="E16" s="8" t="str">
+        <f>window_size_15!B73</f>
+        <v>Yes</v>
+      </c>
+      <c r="F16" s="8" t="str">
+        <f>window_size_15!B96</f>
+        <v>Yes</v>
+      </c>
+      <c r="G16" s="8" t="str">
+        <f>window_size_15!B119</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="7" t="str">
+        <f>window_size_15!B4</f>
+        <v>All</v>
+      </c>
+      <c r="C17" s="7" t="str">
+        <f>window_size_15!B28</f>
+        <v>Is_Gaze_On_Hazard</v>
+      </c>
+      <c r="D17" s="8" t="str">
+        <f>window_size_15!B51</f>
+        <v>Is_Gaze_On_Hazard</v>
+      </c>
+      <c r="E17" s="8" t="str">
+        <f>window_size_15!B74</f>
+        <v>Is_Gaze_On_Hazard</v>
+      </c>
+      <c r="F17" s="8" t="str">
+        <f>window_size_15!B97</f>
+        <v>Is_Gaze_On_Hazard</v>
+      </c>
+      <c r="G17" s="8" t="str">
+        <f>window_size_15!B120</f>
+        <v>Is_Gaze_On_Hazard</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="7">
+        <f>window_size_15!B5</f>
+        <v>31158</v>
+      </c>
+      <c r="C18" s="7">
+        <f>window_size_15!B29</f>
+        <v>31158</v>
+      </c>
+      <c r="D18" s="8">
+        <f>window_size_15!B52</f>
+        <v>31158</v>
+      </c>
+      <c r="E18" s="8">
+        <f>window_size_15!B75</f>
+        <v>59782</v>
+      </c>
+      <c r="F18" s="8">
+        <f>window_size_15!B98</f>
+        <v>31023</v>
+      </c>
+      <c r="G18" s="8">
+        <f>window_size_15!B121</f>
+        <v>31158</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="7">
+        <f>window_size_15!B6</f>
+        <v>0</v>
+      </c>
+      <c r="C19" s="7">
+        <f>window_size_15!B30</f>
+        <v>0</v>
+      </c>
+      <c r="D19" s="8">
+        <f>window_size_15!B53</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="8">
+        <f>window_size_15!B76</f>
+        <v>0</v>
+      </c>
+      <c r="F19" s="8">
+        <f>window_size_15!B99</f>
+        <v>0</v>
+      </c>
+      <c r="G19" s="8">
+        <f>window_size_15!B122</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="7" t="str">
+        <f>window_size_15!B7</f>
+        <v>NAN</v>
+      </c>
+      <c r="C20" s="7">
+        <f>window_size_15!B31</f>
+        <v>0.48458149779735599</v>
+      </c>
+      <c r="D20" s="8">
+        <f>window_size_15!B54</f>
+        <v>0.21401752190237699</v>
+      </c>
+      <c r="E20" s="8">
+        <f>window_size_15!B77</f>
+        <v>0.23137731833384001</v>
+      </c>
+      <c r="F20" s="8">
+        <f>window_size_15!B100</f>
+        <v>0.18088386433710099</v>
+      </c>
+      <c r="G20" s="8">
+        <f>window_size_15!B123</f>
+        <v>0.22007722007722</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="7">
+        <f>window_size_15!B8</f>
+        <v>0</v>
+      </c>
+      <c r="C21" s="7">
+        <f>window_size_15!B32</f>
+        <v>6.7278287461773695E-2</v>
+      </c>
+      <c r="D21" s="8">
+        <f>window_size_15!B55</f>
+        <v>0.10458715596330199</v>
+      </c>
+      <c r="E21" s="8">
+        <f>window_size_15!B78</f>
+        <v>1</v>
+      </c>
+      <c r="F21" s="8">
+        <f>window_size_15!B101</f>
+        <v>0.107645259938837</v>
+      </c>
+      <c r="G21" s="8">
+        <f>window_size_15!B124</f>
+        <v>0.10458715596330199</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="7" t="str">
+        <f>window_size_15!B9</f>
+        <v>NAN</v>
+      </c>
+      <c r="C22" s="7">
+        <f>window_size_15!B33</f>
+        <v>0.118152524167561</v>
+      </c>
+      <c r="D22" s="8">
+        <f>window_size_15!B56</f>
+        <v>0.14050944946589899</v>
+      </c>
+      <c r="E22" s="8">
+        <f>window_size_15!B79</f>
+        <v>0.37580246913580201</v>
+      </c>
+      <c r="F22" s="8">
+        <f>window_size_15!B102</f>
+        <v>0.13496932515337401</v>
+      </c>
+      <c r="G22" s="8">
+        <f>window_size_15!B125</f>
+        <v>0.14179104477611901</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="7">
+        <f>window_size_15!B10</f>
+        <v>0.94752551511650296</v>
+      </c>
+      <c r="C23" s="7">
+        <f>window_size_15!B34</f>
+        <v>0.94730085371333195</v>
+      </c>
+      <c r="D23" s="8">
+        <f>window_size_15!B57</f>
+        <v>0.93285833493805703</v>
+      </c>
+      <c r="E23" s="8">
+        <f>window_size_15!B80</f>
+        <v>0.95771302398715297</v>
+      </c>
+      <c r="F23" s="8">
+        <f>window_size_15!B103</f>
+        <v>0.927594839206624</v>
+      </c>
+      <c r="G23" s="8">
+        <f>window_size_15!B126</f>
+        <v>0.93356441363373699</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="7">
+        <f>window_size_15!B11</f>
+        <v>1</v>
+      </c>
+      <c r="C24" s="7">
+        <f>window_size_15!B35</f>
+        <v>0.99603698811096397</v>
+      </c>
+      <c r="D24" s="8">
+        <f>window_size_15!B58</f>
+        <v>0.97872844900585898</v>
+      </c>
+      <c r="E24" s="8">
+        <f>window_size_15!B81</f>
+        <v>0.95716778773656797</v>
+      </c>
+      <c r="F24" s="8">
+        <f>window_size_15!B104</f>
+        <v>0.973004098499475</v>
+      </c>
+      <c r="G24" s="8">
+        <f>window_size_15!B127</f>
+        <v>0.97947363072858395</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="7">
+        <f>window_size_15!B12</f>
+        <v>0.5</v>
+      </c>
+      <c r="C25" s="7">
+        <f>window_size_15!B36</f>
+        <v>0.53165763778636899</v>
+      </c>
+      <c r="D25" s="8">
+        <f>window_size_15!B59</f>
+        <v>0.54165780248458095</v>
+      </c>
+      <c r="E25" s="8">
+        <f>window_size_15!B82</f>
+        <v>0.97858389386828404</v>
+      </c>
+      <c r="F25" s="8">
+        <f>window_size_15!B105</f>
+        <v>0.54032467921915595</v>
+      </c>
+      <c r="G25" s="8">
+        <f>window_size_15!B128</f>
+        <v>0.54203039334594305</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" s="15" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="12" t="str">
+        <f>window_size_15!B13</f>
+        <v>Test</v>
+      </c>
+      <c r="C26" s="12" t="str">
+        <f>window_size_15!B37</f>
+        <v>Test</v>
+      </c>
+      <c r="D26" s="13" t="str">
+        <f>window_size_15!B60</f>
+        <v>Test</v>
+      </c>
+      <c r="E26" s="13" t="str">
+        <f>window_size_15!B83</f>
+        <v>Validation</v>
+      </c>
+      <c r="F26" s="13" t="str">
+        <f>window_size_15!B106</f>
+        <v>Test</v>
+      </c>
+      <c r="G26" s="13" t="str">
+        <f>window_size_15!B129</f>
+        <v>Test</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" s="19" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="17" t="str">
         <f>window_size_10!B1</f>
         <v>SVM</v>
       </c>
-      <c r="O1" s="4" t="str">
+      <c r="C27" s="17" t="str">
         <f>window_size_10!B25</f>
         <v>SVM</v>
       </c>
-      <c r="P1" s="3" t="str">
+      <c r="D27" s="18" t="str">
         <f>window_size_10!B48</f>
         <v>SVM</v>
       </c>
-      <c r="Q1" s="3" t="str">
+      <c r="E27" s="18" t="str">
         <f>window_size_10!B71</f>
         <v>SVM</v>
       </c>
-      <c r="R1" s="3" t="str">
+      <c r="F27" s="18" t="str">
         <f>window_size_10!B94</f>
         <v>RF</v>
       </c>
-      <c r="S1" s="3" t="str">
+      <c r="G27" s="18" t="str">
         <f>window_size_10!B117</f>
         <v>MLP</v>
       </c>
-      <c r="T1" s="4" t="str">
+    </row>
+    <row r="28" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="7">
+        <f>window_size_10!B2</f>
+        <v>10</v>
+      </c>
+      <c r="C28" s="7">
+        <f>window_size_10!B26</f>
+        <v>10</v>
+      </c>
+      <c r="D28" s="8">
+        <f>window_size_10!B49</f>
+        <v>10</v>
+      </c>
+      <c r="E28" s="8">
+        <f>window_size_10!B72</f>
+        <v>10</v>
+      </c>
+      <c r="F28" s="8">
+        <f>window_size_10!B95</f>
+        <v>10</v>
+      </c>
+      <c r="G28" s="8">
+        <f>window_size_10!B118</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="7" t="str">
+        <f>window_size_10!B3</f>
+        <v>No</v>
+      </c>
+      <c r="C29" s="7" t="str">
+        <f>window_size_10!B27</f>
+        <v>No</v>
+      </c>
+      <c r="D29" s="8" t="str">
+        <f>window_size_10!B50</f>
+        <v>Yes</v>
+      </c>
+      <c r="E29" s="8" t="str">
+        <f>window_size_10!B73</f>
+        <v>Yes</v>
+      </c>
+      <c r="F29" s="8" t="str">
+        <f>window_size_10!B96</f>
+        <v>Yes</v>
+      </c>
+      <c r="G29" s="8" t="str">
+        <f>window_size_10!B119</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30" s="7" t="str">
+        <f>window_size_10!B4</f>
+        <v>All</v>
+      </c>
+      <c r="C30" s="7" t="str">
+        <f>window_size_10!B28</f>
+        <v>Is_Gaze_On_Hazard</v>
+      </c>
+      <c r="D30" s="8" t="str">
+        <f>window_size_10!B51</f>
+        <v>Is_Gaze_On_Hazard</v>
+      </c>
+      <c r="E30" s="8" t="str">
+        <f>window_size_10!B74</f>
+        <v>Is_Gaze_On_Hazard</v>
+      </c>
+      <c r="F30" s="8" t="str">
+        <f>window_size_10!B97</f>
+        <v>Is_Gaze_On_Hazard</v>
+      </c>
+      <c r="G30" s="8" t="str">
+        <f>window_size_10!B120</f>
+        <v>Is_Gaze_On_Hazard</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="7">
+        <f>window_size_10!B5</f>
+        <v>31293</v>
+      </c>
+      <c r="C31" s="7">
+        <f>window_size_10!B29</f>
+        <v>31293</v>
+      </c>
+      <c r="D31" s="8">
+        <f>window_size_10!B52</f>
+        <v>31293</v>
+      </c>
+      <c r="E31" s="8">
+        <f>window_size_10!B75</f>
+        <v>60052</v>
+      </c>
+      <c r="F31" s="8">
+        <f>window_size_10!B98</f>
+        <v>31293</v>
+      </c>
+      <c r="G31" s="8">
+        <f>window_size_10!B121</f>
+        <v>31293</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="7">
+        <f>window_size_10!B6</f>
+        <v>0</v>
+      </c>
+      <c r="C32" s="7">
+        <f>window_size_10!B30</f>
+        <v>0</v>
+      </c>
+      <c r="D32" s="8">
+        <f>window_size_10!B53</f>
+        <v>0</v>
+      </c>
+      <c r="E32" s="8">
+        <f>window_size_10!B76</f>
+        <v>0</v>
+      </c>
+      <c r="F32" s="8">
+        <f>window_size_10!B99</f>
+        <v>0</v>
+      </c>
+      <c r="G32" s="8">
+        <f>window_size_10!B122</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" s="7" t="str">
+        <f>window_size_10!B7</f>
+        <v>NAN</v>
+      </c>
+      <c r="C33" s="7">
+        <f>window_size_10!B31</f>
+        <v>0.43656716417910402</v>
+      </c>
+      <c r="D33" s="8">
+        <f>window_size_10!B54</f>
+        <v>0.19585253456221199</v>
+      </c>
+      <c r="E33" s="8">
+        <f>window_size_10!B77</f>
+        <v>0.22317596566523601</v>
+      </c>
+      <c r="F33" s="8">
+        <f>window_size_10!B100</f>
+        <v>0.16538461538461499</v>
+      </c>
+      <c r="G33" s="8">
+        <f>window_size_10!B123</f>
+        <v>0.18087318087318</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34" s="7">
+        <f>window_size_10!B8</f>
+        <v>0</v>
+      </c>
+      <c r="C34" s="7">
+        <f>window_size_10!B32</f>
+        <v>7.1124620060790206E-2</v>
+      </c>
+      <c r="D34" s="8">
+        <f>window_size_10!B55</f>
+        <v>0.103343465045592</v>
+      </c>
+      <c r="E34" s="8">
+        <f>window_size_10!B78</f>
+        <v>0.99871959026888601</v>
+      </c>
+      <c r="F34" s="8">
+        <f>window_size_10!B101</f>
+        <v>0.104559270516717</v>
+      </c>
+      <c r="G34" s="8">
+        <f>window_size_10!B124</f>
+        <v>0.105775075987841</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" s="7" t="str">
+        <f>window_size_10!B9</f>
+        <v>NAN</v>
+      </c>
+      <c r="C35" s="7">
+        <f>window_size_10!B33</f>
+        <v>0.122320961840041</v>
+      </c>
+      <c r="D35" s="8">
+        <f>window_size_10!B56</f>
+        <v>0.135296458416235</v>
+      </c>
+      <c r="E35" s="8">
+        <f>window_size_10!B79</f>
+        <v>0.364826941066417</v>
+      </c>
+      <c r="F35" s="8">
+        <f>window_size_10!B102</f>
+        <v>0.12811918063314701</v>
+      </c>
+      <c r="G35" s="8">
+        <f>window_size_10!B125</f>
+        <v>0.13348676639815801</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B36" s="7">
+        <f>window_size_10!B10</f>
+        <v>0.94743233310964103</v>
+      </c>
+      <c r="C36" s="7">
+        <f>window_size_10!B34</f>
+        <v>0.94634582814047796</v>
+      </c>
+      <c r="D36" s="8">
+        <f>window_size_10!B57</f>
+        <v>0.93055955005911795</v>
+      </c>
+      <c r="E36" s="8">
+        <f>window_size_10!B80</f>
+        <v>0.95477253047358901</v>
+      </c>
+      <c r="F36" s="8">
+        <f>window_size_10!B103</f>
+        <v>0.92519093727031598</v>
+      </c>
+      <c r="G36" s="8">
+        <f>window_size_10!B126</f>
+        <v>0.92781133160770701</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" s="7">
+        <f>window_size_10!B11</f>
+        <v>1</v>
+      </c>
+      <c r="C37" s="7">
+        <f>window_size_10!B35</f>
+        <v>0.99490690771721502</v>
+      </c>
+      <c r="D37" s="8">
+        <f>window_size_10!B58</f>
+        <v>0.97645709660010704</v>
+      </c>
+      <c r="E37" s="8">
+        <f>window_size_10!B81</f>
+        <v>0.95419345042263504</v>
+      </c>
+      <c r="F37" s="8">
+        <f>window_size_10!B104</f>
+        <v>0.970723151645979</v>
+      </c>
+      <c r="G37" s="8">
+        <f>window_size_10!B127</f>
+        <v>0.97342147868321605</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B38" s="7">
+        <f>window_size_10!B12</f>
+        <v>0.5</v>
+      </c>
+      <c r="C38" s="7">
+        <f>window_size_10!B36</f>
+        <v>0.53301576388900196</v>
+      </c>
+      <c r="D38" s="8">
+        <f>window_size_10!B59</f>
+        <v>0.53990028082285002</v>
+      </c>
+      <c r="E38" s="8">
+        <f>window_size_10!B82</f>
+        <v>0.97645652034576003</v>
+      </c>
+      <c r="F38" s="8">
+        <f>window_size_10!B105</f>
+        <v>0.53764121108134799</v>
+      </c>
+      <c r="G38" s="8">
+        <f>window_size_10!B128</f>
+        <v>0.53959827733552901</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" s="15" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B39" s="12" t="str">
+        <f>window_size_10!B13</f>
+        <v>Test</v>
+      </c>
+      <c r="C39" s="12" t="str">
+        <f>window_size_10!B37</f>
+        <v>Test</v>
+      </c>
+      <c r="D39" s="13" t="str">
+        <f>window_size_10!B60</f>
+        <v>Test</v>
+      </c>
+      <c r="E39" s="13" t="str">
+        <f>window_size_10!B83</f>
+        <v>Validation</v>
+      </c>
+      <c r="F39" s="13" t="str">
+        <f>window_size_10!B106</f>
+        <v>Test</v>
+      </c>
+      <c r="G39" s="13" t="str">
+        <f>window_size_10!B129</f>
+        <v>Test</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40" s="4" t="str">
         <f>window_size_5!B1</f>
         <v>SVM</v>
       </c>
-      <c r="U1" s="4" t="str">
+      <c r="C40" s="4" t="str">
         <f>window_size_5!B25</f>
         <v>SVM</v>
       </c>
-      <c r="V1" s="3" t="str">
+      <c r="D40" s="3" t="str">
         <f>window_size_5!B48</f>
         <v>SVM</v>
       </c>
-      <c r="W1" s="3" t="str">
+      <c r="E40" s="3" t="str">
         <f>window_size_5!B71</f>
         <v>SVM</v>
       </c>
-      <c r="X1" s="3" t="str">
+      <c r="F40" s="3" t="str">
         <f>window_size_5!B94</f>
         <v>RF</v>
       </c>
-      <c r="Y1" s="3" t="str">
+      <c r="G40" s="3" t="str">
         <f>window_size_5!B117</f>
         <v>MLP</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4">
-        <f>window_size_20!B2</f>
-        <v>20</v>
-      </c>
-      <c r="C2" s="4">
-        <f>window_size_20!B26</f>
-        <v>20</v>
-      </c>
-      <c r="D2" s="3">
-        <f>window_size_20!B49</f>
-        <v>20</v>
-      </c>
-      <c r="E2" s="3">
-        <f>window_size_20!B72</f>
-        <v>20</v>
-      </c>
-      <c r="F2" s="3">
-        <f>window_size_20!B95</f>
-        <v>20</v>
-      </c>
-      <c r="G2" s="3">
-        <f>window_size_20!B118</f>
-        <v>20</v>
-      </c>
-      <c r="H2" s="4">
-        <f>window_size_15!B2</f>
-        <v>15</v>
-      </c>
-      <c r="I2" s="4">
-        <f>window_size_15!B26</f>
-        <v>15</v>
-      </c>
-      <c r="J2" s="3">
-        <f>window_size_15!B49</f>
-        <v>15</v>
-      </c>
-      <c r="K2" s="3">
-        <f>window_size_15!B72</f>
-        <v>15</v>
-      </c>
-      <c r="L2" s="3">
-        <f>window_size_15!B95</f>
-        <v>15</v>
-      </c>
-      <c r="M2" s="3">
-        <f>window_size_15!B118</f>
-        <v>15</v>
-      </c>
-      <c r="N2" s="4">
-        <f>window_size_10!B2</f>
-        <v>10</v>
-      </c>
-      <c r="O2" s="4">
-        <f>window_size_10!B26</f>
-        <v>10</v>
-      </c>
-      <c r="P2" s="3">
-        <f>window_size_10!B49</f>
-        <v>10</v>
-      </c>
-      <c r="Q2" s="3">
-        <f>window_size_10!B72</f>
-        <v>10</v>
-      </c>
-      <c r="R2" s="3">
-        <f>window_size_10!B95</f>
-        <v>10</v>
-      </c>
-      <c r="S2" s="3">
-        <f>window_size_10!B118</f>
-        <v>10</v>
-      </c>
-      <c r="T2" s="4">
+      <c r="B41" s="4">
         <f>window_size_5!B2</f>
         <v>5</v>
       </c>
-      <c r="U2" s="4">
+      <c r="C41" s="4">
         <f>window_size_5!B26</f>
         <v>5</v>
       </c>
-      <c r="V2" s="3">
+      <c r="D41" s="3">
         <f>window_size_5!B49</f>
         <v>5</v>
       </c>
-      <c r="W2" s="3">
+      <c r="E41" s="3">
         <f>window_size_5!B72</f>
         <v>5</v>
       </c>
-      <c r="X2" s="3">
+      <c r="F41" s="3">
         <f>window_size_5!B95</f>
         <v>5</v>
       </c>
-      <c r="Y2" s="3">
+      <c r="G41" s="3">
         <f>window_size_5!B118</f>
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="str">
-        <f>window_size_20!B3</f>
-        <v>No</v>
-      </c>
-      <c r="C3" s="4" t="str">
-        <f>window_size_20!B27</f>
-        <v>No</v>
-      </c>
-      <c r="D3" s="3" t="str">
-        <f>window_size_20!B50</f>
-        <v>Yes</v>
-      </c>
-      <c r="E3" s="3" t="str">
-        <f>window_size_20!B73</f>
-        <v>Yes</v>
-      </c>
-      <c r="F3" s="3" t="str">
-        <f>window_size_20!B96</f>
-        <v>Yes</v>
-      </c>
-      <c r="G3" s="3" t="str">
-        <f>window_size_20!B119</f>
-        <v>Yes</v>
-      </c>
-      <c r="H3" s="4" t="str">
-        <f>window_size_15!B3</f>
-        <v>No</v>
-      </c>
-      <c r="I3" s="4" t="str">
-        <f>window_size_15!B27</f>
-        <v>No</v>
-      </c>
-      <c r="J3" s="3" t="str">
-        <f>window_size_15!B50</f>
-        <v>Yes</v>
-      </c>
-      <c r="K3" s="3" t="str">
-        <f>window_size_15!B73</f>
-        <v>Yes</v>
-      </c>
-      <c r="L3" s="3" t="str">
-        <f>window_size_15!B96</f>
-        <v>Yes</v>
-      </c>
-      <c r="M3" s="3" t="str">
-        <f>window_size_15!B119</f>
-        <v>Yes</v>
-      </c>
-      <c r="N3" s="4" t="str">
-        <f>window_size_10!B3</f>
-        <v>No</v>
-      </c>
-      <c r="O3" s="4" t="str">
-        <f>window_size_10!B27</f>
-        <v>No</v>
-      </c>
-      <c r="P3" s="3" t="str">
-        <f>window_size_10!B50</f>
-        <v>Yes</v>
-      </c>
-      <c r="Q3" s="3" t="str">
-        <f>window_size_10!B73</f>
-        <v>Yes</v>
-      </c>
-      <c r="R3" s="3" t="str">
-        <f>window_size_10!B96</f>
-        <v>Yes</v>
-      </c>
-      <c r="S3" s="3" t="str">
-        <f>window_size_10!B119</f>
-        <v>Yes</v>
-      </c>
-      <c r="T3" s="4" t="str">
+      <c r="B42" s="4" t="str">
         <f>window_size_5!B3</f>
         <v>No</v>
       </c>
-      <c r="U3" s="4" t="str">
+      <c r="C42" s="4" t="str">
         <f>window_size_5!B27</f>
         <v>No</v>
       </c>
-      <c r="V3" s="3" t="str">
+      <c r="D42" s="3" t="str">
         <f>window_size_5!B50</f>
         <v>Yes</v>
       </c>
-      <c r="W3" s="3" t="str">
+      <c r="E42" s="3" t="str">
         <f>window_size_5!B73</f>
         <v>Yes</v>
       </c>
-      <c r="X3" s="3" t="str">
+      <c r="F42" s="3" t="str">
         <f>window_size_5!B96</f>
         <v>Yes</v>
       </c>
-      <c r="Y3" s="3" t="str">
+      <c r="G42" s="3" t="str">
         <f>window_size_5!B119</f>
         <v>Yes</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="str">
-        <f>window_size_20!B4</f>
-        <v>All</v>
-      </c>
-      <c r="C4" s="4" t="str">
-        <f>window_size_20!B28</f>
-        <v>Is_Gaze_On_Hazard</v>
-      </c>
-      <c r="D4" s="3" t="str">
-        <f>window_size_20!B51</f>
-        <v>Is_Gaze_On_Hazard</v>
-      </c>
-      <c r="E4" s="3" t="str">
-        <f>window_size_20!B74</f>
-        <v>Is_Gaze_On_Hazard</v>
-      </c>
-      <c r="F4" s="3" t="str">
-        <f>window_size_20!B97</f>
-        <v>Is_Gaze_On_Hazard</v>
-      </c>
-      <c r="G4" s="3" t="str">
-        <f>window_size_20!B120</f>
-        <v>Is_Gaze_On_Hazard</v>
-      </c>
-      <c r="H4" s="4" t="str">
-        <f>window_size_15!B4</f>
-        <v>All</v>
-      </c>
-      <c r="I4" s="4" t="str">
-        <f>window_size_15!B28</f>
-        <v>Is_Gaze_On_Hazard</v>
-      </c>
-      <c r="J4" s="3" t="str">
-        <f>window_size_15!B51</f>
-        <v>Is_Gaze_On_Hazard</v>
-      </c>
-      <c r="K4" s="3" t="str">
-        <f>window_size_15!B74</f>
-        <v>Is_Gaze_On_Hazard</v>
-      </c>
-      <c r="L4" s="3" t="str">
-        <f>window_size_15!B97</f>
-        <v>Is_Gaze_On_Hazard</v>
-      </c>
-      <c r="M4" s="3" t="str">
-        <f>window_size_15!B120</f>
-        <v>Is_Gaze_On_Hazard</v>
-      </c>
-      <c r="N4" s="4" t="str">
-        <f>window_size_10!B4</f>
-        <v>All</v>
-      </c>
-      <c r="O4" s="4" t="str">
-        <f>window_size_10!B28</f>
-        <v>Is_Gaze_On_Hazard</v>
-      </c>
-      <c r="P4" s="3" t="str">
-        <f>window_size_10!B51</f>
-        <v>Is_Gaze_On_Hazard</v>
-      </c>
-      <c r="Q4" s="3" t="str">
-        <f>window_size_10!B74</f>
-        <v>Is_Gaze_On_Hazard</v>
-      </c>
-      <c r="R4" s="3" t="str">
-        <f>window_size_10!B97</f>
-        <v>Is_Gaze_On_Hazard</v>
-      </c>
-      <c r="S4" s="3" t="str">
-        <f>window_size_10!B120</f>
-        <v>Is_Gaze_On_Hazard</v>
-      </c>
-      <c r="T4" s="4" t="str">
+      <c r="B43" s="4" t="str">
         <f>window_size_5!B4</f>
         <v>All</v>
       </c>
-      <c r="U4" s="4" t="str">
+      <c r="C43" s="4" t="str">
         <f>window_size_5!B28</f>
         <v>Is_Gaze_On_Hazard</v>
       </c>
-      <c r="V4" s="3" t="str">
+      <c r="D43" s="3" t="str">
         <f>window_size_5!B51</f>
         <v>Is_Gaze_On_Hazard</v>
       </c>
-      <c r="W4" s="3" t="str">
+      <c r="E43" s="3" t="str">
         <f>window_size_5!B74</f>
         <v>Is_Gaze_On_Hazard</v>
       </c>
-      <c r="X4" s="3" t="str">
+      <c r="F43" s="3" t="str">
         <f>window_size_5!B97</f>
         <v>Is_Gaze_On_Hazard</v>
       </c>
-      <c r="Y4" s="3" t="str">
+      <c r="G43" s="3" t="str">
         <f>window_size_5!B120</f>
         <v>Is_Gaze_On_Hazard</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="4">
-        <f>window_size_20!B5</f>
-        <v>31023</v>
-      </c>
-      <c r="C5" s="4">
-        <f>window_size_20!B29</f>
-        <v>31023</v>
-      </c>
-      <c r="D5" s="3">
-        <f>window_size_20!B52</f>
-        <v>31023</v>
-      </c>
-      <c r="E5" s="3">
-        <f>window_size_20!B75</f>
-        <v>59512</v>
-      </c>
-      <c r="F5" s="3">
-        <f>window_size_20!B98</f>
-        <v>31023</v>
-      </c>
-      <c r="G5" s="3">
-        <f>window_size_20!B121</f>
-        <v>31023</v>
-      </c>
-      <c r="H5" s="4">
-        <f>window_size_15!B5</f>
-        <v>31158</v>
-      </c>
-      <c r="I5" s="4">
-        <f>window_size_15!B29</f>
-        <v>31158</v>
-      </c>
-      <c r="J5" s="3">
-        <f>window_size_15!B52</f>
-        <v>31158</v>
-      </c>
-      <c r="K5" s="3">
-        <f>window_size_15!B75</f>
-        <v>59782</v>
-      </c>
-      <c r="L5" s="3">
-        <f>window_size_15!B98</f>
-        <v>31023</v>
-      </c>
-      <c r="M5" s="3">
-        <f>window_size_15!B121</f>
-        <v>31158</v>
-      </c>
-      <c r="N5" s="4">
-        <f>window_size_10!B5</f>
-        <v>31293</v>
-      </c>
-      <c r="O5" s="4">
-        <f>window_size_10!B29</f>
-        <v>31293</v>
-      </c>
-      <c r="P5" s="3">
-        <f>window_size_10!B52</f>
-        <v>31293</v>
-      </c>
-      <c r="Q5" s="3">
-        <f>window_size_10!B75</f>
-        <v>60052</v>
-      </c>
-      <c r="R5" s="3">
-        <f>window_size_10!B98</f>
-        <v>31293</v>
-      </c>
-      <c r="S5" s="3">
-        <f>window_size_10!B121</f>
-        <v>31293</v>
-      </c>
-      <c r="T5" s="4">
+      <c r="B44" s="4">
         <f>window_size_5!B5</f>
         <v>31428</v>
       </c>
-      <c r="U5" s="4">
+      <c r="C44" s="4">
         <f>window_size_5!B29</f>
         <v>31428</v>
       </c>
-      <c r="V5" s="3">
+      <c r="D44" s="3">
         <f>window_size_5!B52</f>
         <v>31428</v>
       </c>
-      <c r="W5" s="3">
+      <c r="E44" s="3">
         <f>window_size_5!B75</f>
         <v>60332</v>
       </c>
-      <c r="X5" s="3">
+      <c r="F44" s="3">
         <f>window_size_5!B98</f>
         <v>31428</v>
       </c>
-      <c r="Y5" s="3">
+      <c r="G44" s="3">
         <f>window_size_5!B121</f>
         <v>31428</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="4">
-        <f>window_size_20!B6</f>
-        <v>0</v>
-      </c>
-      <c r="C6" s="4">
-        <f>window_size_20!B30</f>
-        <v>0</v>
-      </c>
-      <c r="D6" s="3">
-        <f>window_size_20!B53</f>
-        <v>0</v>
-      </c>
-      <c r="E6" s="3">
-        <f>window_size_20!B76</f>
-        <v>0</v>
-      </c>
-      <c r="F6" s="3">
-        <f>window_size_20!B99</f>
-        <v>0</v>
-      </c>
-      <c r="G6" s="3">
-        <f>window_size_20!B122</f>
-        <v>0</v>
-      </c>
-      <c r="H6" s="4">
-        <f>window_size_15!B6</f>
-        <v>0</v>
-      </c>
-      <c r="I6" s="4">
-        <f>window_size_15!B30</f>
-        <v>0</v>
-      </c>
-      <c r="J6" s="3">
-        <f>window_size_15!B53</f>
-        <v>0</v>
-      </c>
-      <c r="K6" s="3">
-        <f>window_size_15!B76</f>
-        <v>0</v>
-      </c>
-      <c r="L6" s="3">
-        <f>window_size_15!B99</f>
-        <v>0</v>
-      </c>
-      <c r="M6" s="3">
-        <f>window_size_15!B122</f>
-        <v>0</v>
-      </c>
-      <c r="N6" s="4">
-        <f>window_size_10!B6</f>
-        <v>0</v>
-      </c>
-      <c r="O6" s="4">
-        <f>window_size_10!B30</f>
-        <v>0</v>
-      </c>
-      <c r="P6" s="3">
-        <f>window_size_10!B53</f>
-        <v>0</v>
-      </c>
-      <c r="Q6" s="3">
-        <f>window_size_10!B76</f>
-        <v>0</v>
-      </c>
-      <c r="R6" s="3">
-        <f>window_size_10!B99</f>
-        <v>0</v>
-      </c>
-      <c r="S6" s="3">
-        <f>window_size_10!B122</f>
-        <v>0</v>
-      </c>
-      <c r="T6" s="4">
+      <c r="B45" s="4">
         <f>window_size_5!B6</f>
         <v>0</v>
       </c>
-      <c r="U6" s="4">
+      <c r="C45" s="4">
         <f>window_size_5!B30</f>
         <v>0</v>
       </c>
-      <c r="V6" s="3">
+      <c r="D45" s="3">
         <f>window_size_5!B53</f>
         <v>0</v>
       </c>
-      <c r="W6" s="3">
+      <c r="E45" s="3">
         <f>window_size_5!B76</f>
         <v>0</v>
       </c>
-      <c r="X6" s="3">
+      <c r="F45" s="3">
         <f>window_size_5!B99</f>
         <v>0</v>
       </c>
-      <c r="Y6" s="3">
+      <c r="G45" s="3">
         <f>window_size_5!B122</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="4" t="str">
-        <f>window_size_20!B7</f>
-        <v>NAN</v>
-      </c>
-      <c r="C7" s="4">
-        <f>window_size_20!B31</f>
-        <v>0.50731707317073105</v>
-      </c>
-      <c r="D7" s="3">
-        <f>window_size_20!B54</f>
-        <v>0.206561360874848</v>
-      </c>
-      <c r="E7" s="3">
-        <f>window_size_20!B77</f>
-        <v>0.231634885901844</v>
-      </c>
-      <c r="F7" s="3">
-        <f>window_size_20!B100</f>
-        <v>0.19160387513455299</v>
-      </c>
-      <c r="G7" s="3">
-        <f>window_size_20!B123</f>
-        <v>0.223188405797101</v>
-      </c>
-      <c r="H7" s="4" t="str">
-        <f>window_size_15!B7</f>
-        <v>NAN</v>
-      </c>
-      <c r="I7" s="4">
-        <f>window_size_15!B31</f>
-        <v>0.48458149779735599</v>
-      </c>
-      <c r="J7" s="3">
-        <f>window_size_15!B54</f>
-        <v>0.21401752190237699</v>
-      </c>
-      <c r="K7" s="3">
-        <f>window_size_15!B77</f>
-        <v>0.23137731833384001</v>
-      </c>
-      <c r="L7" s="3">
-        <f>window_size_15!B100</f>
-        <v>0.18088386433710099</v>
-      </c>
-      <c r="M7" s="3">
-        <f>window_size_15!B123</f>
-        <v>0.22007722007722</v>
-      </c>
-      <c r="N7" s="4" t="str">
-        <f>window_size_10!B7</f>
-        <v>NAN</v>
-      </c>
-      <c r="O7" s="4">
-        <f>window_size_10!B31</f>
-        <v>0.43656716417910402</v>
-      </c>
-      <c r="P7" s="3">
-        <f>window_size_10!B54</f>
-        <v>0.19585253456221199</v>
-      </c>
-      <c r="Q7" s="3">
-        <f>window_size_10!B77</f>
-        <v>0.22317596566523601</v>
-      </c>
-      <c r="R7" s="3">
-        <f>window_size_10!B100</f>
-        <v>0.16538461538461499</v>
-      </c>
-      <c r="S7" s="3">
-        <f>window_size_10!B123</f>
-        <v>0.18087318087318</v>
-      </c>
-      <c r="T7" s="4" t="str">
+      <c r="B46" s="4" t="str">
         <f>window_size_5!B7</f>
         <v>NAN</v>
       </c>
-      <c r="U7" s="4">
+      <c r="C46" s="4">
         <f>window_size_5!B31</f>
         <v>0.38165680473372698</v>
       </c>
-      <c r="V7" s="3">
+      <c r="D46" s="3">
         <f>window_size_5!B54</f>
         <v>0.158730158730158</v>
       </c>
-      <c r="W7" s="3">
+      <c r="E46" s="3">
         <f>window_size_5!B77</f>
         <v>0.19939879759519</v>
       </c>
-      <c r="X7" s="3">
+      <c r="F46" s="3">
         <f>window_size_5!B100</f>
         <v>0.14380714879467901</v>
       </c>
-      <c r="Y7" s="3">
+      <c r="G46" s="3">
         <f>window_size_5!B123</f>
         <v>0.16867469879517999</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="4">
-        <f>window_size_20!B8</f>
-        <v>0</v>
-      </c>
-      <c r="C8" s="4">
-        <f>window_size_20!B32</f>
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="D8" s="3">
-        <f>window_size_20!B55</f>
-        <v>0.104615384615384</v>
-      </c>
-      <c r="E8" s="3">
-        <f>window_size_20!B78</f>
-        <v>1</v>
-      </c>
-      <c r="F8" s="3">
-        <f>window_size_20!B101</f>
-        <v>0.109538461538461</v>
-      </c>
-      <c r="G8" s="3">
-        <f>window_size_20!B124</f>
-        <v>9.4769230769230703E-2</v>
-      </c>
-      <c r="H8" s="4">
-        <f>window_size_15!B8</f>
-        <v>0</v>
-      </c>
-      <c r="I8" s="4">
-        <f>window_size_15!B32</f>
-        <v>6.7278287461773695E-2</v>
-      </c>
-      <c r="J8" s="3">
-        <f>window_size_15!B55</f>
-        <v>0.10458715596330199</v>
-      </c>
-      <c r="K8" s="3">
-        <f>window_size_15!B78</f>
-        <v>1</v>
-      </c>
-      <c r="L8" s="3">
-        <f>window_size_15!B101</f>
-        <v>0.107645259938837</v>
-      </c>
-      <c r="M8" s="3">
-        <f>window_size_15!B124</f>
-        <v>0.10458715596330199</v>
-      </c>
-      <c r="N8" s="4">
-        <f>window_size_10!B8</f>
-        <v>0</v>
-      </c>
-      <c r="O8" s="4">
-        <f>window_size_10!B32</f>
-        <v>7.1124620060790206E-2</v>
-      </c>
-      <c r="P8" s="3">
-        <f>window_size_10!B55</f>
-        <v>0.103343465045592</v>
-      </c>
-      <c r="Q8" s="3">
-        <f>window_size_10!B78</f>
-        <v>0.99871959026888601</v>
-      </c>
-      <c r="R8" s="3">
-        <f>window_size_10!B101</f>
-        <v>0.104559270516717</v>
-      </c>
-      <c r="S8" s="3">
-        <f>window_size_10!B124</f>
-        <v>0.105775075987841</v>
-      </c>
-      <c r="T8" s="4">
+      <c r="B47" s="4">
         <f>window_size_5!B8</f>
         <v>0</v>
       </c>
-      <c r="U8" s="4">
+      <c r="C47" s="4">
         <f>window_size_5!B32</f>
         <v>7.7945619335347396E-2</v>
       </c>
-      <c r="V8" s="3">
+      <c r="D47" s="3">
         <f>window_size_5!B55</f>
         <v>0.102719033232628</v>
       </c>
-      <c r="W8" s="3">
+      <c r="E47" s="3">
         <f>window_size_5!B78</f>
         <v>0.993757802746566</v>
       </c>
-      <c r="X8" s="3">
+      <c r="F47" s="3">
         <f>window_size_5!B101</f>
         <v>0.10453172205437999</v>
       </c>
-      <c r="Y8" s="3">
+      <c r="G47" s="3">
         <f>window_size_5!B124</f>
         <v>0.10151057401812601</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="4" t="str">
-        <f>window_size_20!B9</f>
-        <v>NAN</v>
-      </c>
-      <c r="C9" s="4">
-        <f>window_size_20!B33</f>
-        <v>0.113661202185792</v>
-      </c>
-      <c r="D9" s="3">
-        <f>window_size_20!B56</f>
-        <v>0.13888888888888801</v>
-      </c>
-      <c r="E9" s="3">
-        <f>window_size_20!B79</f>
-        <v>0.37614213197969498</v>
-      </c>
-      <c r="F9" s="3">
-        <f>window_size_20!B102</f>
-        <v>0.139389193422083</v>
-      </c>
-      <c r="G9" s="3">
-        <f>window_size_20!B125</f>
-        <v>0.13304535637149001</v>
-      </c>
-      <c r="H9" s="4" t="str">
-        <f>window_size_15!B9</f>
-        <v>NAN</v>
-      </c>
-      <c r="I9" s="4">
-        <f>window_size_15!B33</f>
-        <v>0.118152524167561</v>
-      </c>
-      <c r="J9" s="3">
-        <f>window_size_15!B56</f>
-        <v>0.14050944946589899</v>
-      </c>
-      <c r="K9" s="3">
-        <f>window_size_15!B79</f>
-        <v>0.37580246913580201</v>
-      </c>
-      <c r="L9" s="3">
-        <f>window_size_15!B102</f>
-        <v>0.13496932515337401</v>
-      </c>
-      <c r="M9" s="3">
-        <f>window_size_15!B125</f>
-        <v>0.14179104477611901</v>
-      </c>
-      <c r="N9" s="4" t="str">
-        <f>window_size_10!B9</f>
-        <v>NAN</v>
-      </c>
-      <c r="O9" s="4">
-        <f>window_size_10!B33</f>
-        <v>0.122320961840041</v>
-      </c>
-      <c r="P9" s="3">
-        <f>window_size_10!B56</f>
-        <v>0.135296458416235</v>
-      </c>
-      <c r="Q9" s="3">
-        <f>window_size_10!B79</f>
-        <v>0.364826941066417</v>
-      </c>
-      <c r="R9" s="3">
-        <f>window_size_10!B102</f>
-        <v>0.12811918063314701</v>
-      </c>
-      <c r="S9" s="3">
-        <f>window_size_10!B125</f>
-        <v>0.13348676639815801</v>
-      </c>
-      <c r="T9" s="4" t="str">
+      <c r="B48" s="4" t="str">
         <f>window_size_5!B9</f>
         <v>NAN</v>
       </c>
-      <c r="U9" s="4">
+      <c r="C48" s="4">
         <f>window_size_5!B33</f>
         <v>0.12945308580030099</v>
       </c>
-      <c r="V9" s="3">
+      <c r="D48" s="3">
         <f>window_size_5!B56</f>
         <v>0.124724871606749</v>
       </c>
-      <c r="W9" s="3">
+      <c r="E48" s="3">
         <f>window_size_5!B79</f>
         <v>0.33215105361986202</v>
       </c>
-      <c r="X9" s="3">
+      <c r="F48" s="3">
         <f>window_size_5!B102</f>
         <v>0.121063680895731</v>
       </c>
-      <c r="Y9" s="3">
+      <c r="G48" s="3">
         <f>window_size_5!B125</f>
         <v>0.126744624669935</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="4">
-        <f>window_size_20!B10</f>
-        <v>0.947619508106888</v>
-      </c>
-      <c r="C10" s="4">
-        <f>window_size_20!B34</f>
-        <v>0.94771621055346</v>
-      </c>
-      <c r="D10" s="3">
-        <f>window_size_20!B57</f>
-        <v>0.93205041420881196</v>
-      </c>
-      <c r="E10" s="3">
-        <f>window_size_20!B80</f>
-        <v>0.95869740556526395</v>
-      </c>
-      <c r="F10" s="3">
-        <f>window_size_20!B103</f>
-        <v>0.92914934081165501</v>
-      </c>
-      <c r="G10" s="3">
-        <f>window_size_20!B126</f>
-        <v>0.93530606324340004</v>
-      </c>
-      <c r="H10" s="4">
-        <f>window_size_15!B10</f>
-        <v>0.94752551511650296</v>
-      </c>
-      <c r="I10" s="4">
-        <f>window_size_15!B34</f>
-        <v>0.94730085371333195</v>
-      </c>
-      <c r="J10" s="3">
-        <f>window_size_15!B57</f>
-        <v>0.93285833493805703</v>
-      </c>
-      <c r="K10" s="3">
-        <f>window_size_15!B80</f>
-        <v>0.95771302398715297</v>
-      </c>
-      <c r="L10" s="3">
-        <f>window_size_15!B103</f>
-        <v>0.927594839206624</v>
-      </c>
-      <c r="M10" s="3">
-        <f>window_size_15!B126</f>
-        <v>0.93356441363373699</v>
-      </c>
-      <c r="N10" s="4">
-        <f>window_size_10!B10</f>
-        <v>0.94743233310964103</v>
-      </c>
-      <c r="O10" s="4">
-        <f>window_size_10!B34</f>
-        <v>0.94634582814047796</v>
-      </c>
-      <c r="P10" s="3">
-        <f>window_size_10!B57</f>
-        <v>0.93055955005911795</v>
-      </c>
-      <c r="Q10" s="3">
-        <f>window_size_10!B80</f>
-        <v>0.95477253047358901</v>
-      </c>
-      <c r="R10" s="3">
-        <f>window_size_10!B103</f>
-        <v>0.92519093727031598</v>
-      </c>
-      <c r="S10" s="3">
-        <f>window_size_10!B126</f>
-        <v>0.92781133160770701</v>
-      </c>
-      <c r="T10" s="4">
+      <c r="B49" s="4">
         <f>window_size_5!B10</f>
         <v>0.94733995163548401</v>
       </c>
-      <c r="U10" s="4">
+      <c r="C49" s="4">
         <f>window_size_5!B34</f>
         <v>0.94479445080819602</v>
       </c>
-      <c r="V10" s="3">
+      <c r="D49" s="3">
         <f>window_size_5!B57</f>
         <v>0.92408043782614202</v>
       </c>
-      <c r="W10" s="3">
+      <c r="E49" s="3">
         <f>window_size_5!B80</f>
         <v>0.94693478332946501</v>
       </c>
-      <c r="X10" s="3">
+      <c r="F49" s="3">
         <f>window_size_5!B103</f>
         <v>0.92007127402316402</v>
       </c>
-      <c r="Y10" s="3">
+      <c r="G49" s="3">
         <f>window_size_5!B126</f>
         <v>0.92633956981036003</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="4">
-        <f>window_size_20!B11</f>
-        <v>1</v>
-      </c>
-      <c r="C11" s="4">
-        <f>window_size_20!B35</f>
-        <v>0.99656439213551895</v>
-      </c>
-      <c r="D11" s="3">
-        <f>window_size_20!B58</f>
-        <v>0.97778760459895198</v>
-      </c>
-      <c r="E11" s="3">
-        <f>window_size_20!B81</f>
-        <v>0.95817665175001199</v>
-      </c>
-      <c r="F11" s="3">
-        <f>window_size_20!B104</f>
-        <v>0.97445404449282202</v>
-      </c>
-      <c r="G11" s="3">
-        <f>window_size_20!B127</f>
-        <v>0.98176746717463703</v>
-      </c>
-      <c r="H11" s="4">
-        <f>window_size_15!B11</f>
-        <v>1</v>
-      </c>
-      <c r="I11" s="4">
-        <f>window_size_15!B35</f>
-        <v>0.99603698811096397</v>
-      </c>
-      <c r="J11" s="3">
-        <f>window_size_15!B58</f>
-        <v>0.97872844900585898</v>
-      </c>
-      <c r="K11" s="3">
-        <f>window_size_15!B81</f>
-        <v>0.95716778773656797</v>
-      </c>
-      <c r="L11" s="3">
-        <f>window_size_15!B104</f>
-        <v>0.973004098499475</v>
-      </c>
-      <c r="M11" s="3">
-        <f>window_size_15!B127</f>
-        <v>0.97947363072858395</v>
-      </c>
-      <c r="N11" s="4">
-        <f>window_size_10!B11</f>
-        <v>1</v>
-      </c>
-      <c r="O11" s="4">
-        <f>window_size_10!B35</f>
-        <v>0.99490690771721502</v>
-      </c>
-      <c r="P11" s="3">
-        <f>window_size_10!B58</f>
-        <v>0.97645709660010704</v>
-      </c>
-      <c r="Q11" s="3">
-        <f>window_size_10!B81</f>
-        <v>0.95419345042263504</v>
-      </c>
-      <c r="R11" s="3">
-        <f>window_size_10!B104</f>
-        <v>0.970723151645979</v>
-      </c>
-      <c r="S11" s="3">
-        <f>window_size_10!B127</f>
-        <v>0.97342147868321605</v>
-      </c>
-      <c r="T11" s="4">
+      <c r="B50" s="4">
         <f>window_size_5!B11</f>
         <v>1</v>
       </c>
-      <c r="U11" s="4">
+      <c r="C50" s="4">
         <f>window_size_5!B35</f>
         <v>0.99298021697511096</v>
       </c>
-      <c r="V11" s="3">
+      <c r="D50" s="3">
         <f>window_size_5!B58</f>
         <v>0.96973768179222697</v>
       </c>
-      <c r="W11" s="3">
+      <c r="E50" s="3">
         <f>window_size_5!B81</f>
         <v>0.94630466558021498</v>
       </c>
-      <c r="X11" s="3">
+      <c r="F50" s="3">
         <f>window_size_5!B104</f>
         <v>0.96540489705437804</v>
       </c>
-      <c r="Y11" s="3">
+      <c r="G50" s="3">
         <f>window_size_5!B127</f>
         <v>0.97218956772914999</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="4">
-        <f>window_size_20!B12</f>
-        <v>0.5</v>
-      </c>
-      <c r="C12" s="4">
-        <f>window_size_20!B36</f>
-        <v>0.53028219606775895</v>
-      </c>
-      <c r="D12" s="3">
-        <f>window_size_20!B59</f>
-        <v>0.54120149460716804</v>
-      </c>
-      <c r="E12" s="3">
-        <f>window_size_20!B82</f>
-        <v>0.97908832587500605</v>
-      </c>
-      <c r="F12" s="3">
-        <f>window_size_20!B105</f>
-        <v>0.54199625301564203</v>
-      </c>
-      <c r="G12" s="3">
-        <f>window_size_20!B128</f>
-        <v>0.53826834897193399</v>
-      </c>
-      <c r="H12" s="4">
-        <f>window_size_15!B12</f>
-        <v>0.5</v>
-      </c>
-      <c r="I12" s="4">
-        <f>window_size_15!B36</f>
-        <v>0.53165763778636899</v>
-      </c>
-      <c r="J12" s="3">
-        <f>window_size_15!B59</f>
-        <v>0.54165780248458095</v>
-      </c>
-      <c r="K12" s="3">
-        <f>window_size_15!B82</f>
-        <v>0.97858389386828404</v>
-      </c>
-      <c r="L12" s="3">
-        <f>window_size_15!B105</f>
-        <v>0.54032467921915595</v>
-      </c>
-      <c r="M12" s="3">
-        <f>window_size_15!B128</f>
-        <v>0.54203039334594305</v>
-      </c>
-      <c r="N12" s="4">
-        <f>window_size_10!B12</f>
-        <v>0.5</v>
-      </c>
-      <c r="O12" s="4">
-        <f>window_size_10!B36</f>
-        <v>0.53301576388900196</v>
-      </c>
-      <c r="P12" s="3">
-        <f>window_size_10!B59</f>
-        <v>0.53990028082285002</v>
-      </c>
-      <c r="Q12" s="3">
-        <f>window_size_10!B82</f>
-        <v>0.97645652034576003</v>
-      </c>
-      <c r="R12" s="3">
-        <f>window_size_10!B105</f>
-        <v>0.53764121108134799</v>
-      </c>
-      <c r="S12" s="3">
-        <f>window_size_10!B128</f>
-        <v>0.53959827733552901</v>
-      </c>
-      <c r="T12" s="4">
+      <c r="B51" s="4">
         <f>window_size_5!B12</f>
         <v>0.5</v>
       </c>
-      <c r="U12" s="4">
+      <c r="C51" s="4">
         <f>window_size_5!B36</f>
         <v>0.53546291815522895</v>
       </c>
-      <c r="V12" s="3">
+      <c r="D51" s="3">
         <f>window_size_5!B59</f>
         <v>0.53622835751242803</v>
       </c>
-      <c r="W12" s="3">
+      <c r="E51" s="3">
         <f>window_size_5!B82</f>
         <v>0.97003123416339099</v>
       </c>
-      <c r="X12" s="3">
+      <c r="F51" s="3">
         <f>window_size_5!B105</f>
         <v>0.53496830955437902</v>
       </c>
-      <c r="Y12" s="3">
+      <c r="G51" s="3">
         <f>window_size_5!B128</f>
         <v>0.53685007087363801</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="4" t="str">
-        <f>window_size_20!B13</f>
-        <v>Test</v>
-      </c>
-      <c r="C13" s="4" t="str">
-        <f>window_size_20!B37</f>
-        <v>Test</v>
-      </c>
-      <c r="D13" s="3" t="str">
-        <f>window_size_20!B60</f>
-        <v>Test</v>
-      </c>
-      <c r="E13" s="3" t="str">
-        <f>window_size_20!B83</f>
-        <v>Validation</v>
-      </c>
-      <c r="F13" s="3" t="str">
-        <f>window_size_20!B106</f>
-        <v>Test</v>
-      </c>
-      <c r="G13" s="3" t="str">
-        <f>window_size_20!B129</f>
-        <v>Test</v>
-      </c>
-      <c r="H13" s="4" t="str">
-        <f>window_size_15!B13</f>
-        <v>Test</v>
-      </c>
-      <c r="I13" s="4" t="str">
-        <f>window_size_15!B37</f>
-        <v>Test</v>
-      </c>
-      <c r="J13" s="3" t="str">
-        <f>window_size_15!B60</f>
-        <v>Test</v>
-      </c>
-      <c r="K13" s="3" t="str">
-        <f>window_size_15!B83</f>
-        <v>Validation</v>
-      </c>
-      <c r="L13" s="3" t="str">
-        <f>window_size_15!B106</f>
-        <v>Test</v>
-      </c>
-      <c r="M13" s="3" t="str">
-        <f>window_size_15!B129</f>
-        <v>Test</v>
-      </c>
-      <c r="N13" s="4" t="str">
-        <f>window_size_10!B13</f>
-        <v>Test</v>
-      </c>
-      <c r="O13" s="4" t="str">
-        <f>window_size_10!B37</f>
-        <v>Test</v>
-      </c>
-      <c r="P13" s="3" t="str">
-        <f>window_size_10!B60</f>
-        <v>Test</v>
-      </c>
-      <c r="Q13" s="3" t="str">
-        <f>window_size_10!B83</f>
-        <v>Validation</v>
-      </c>
-      <c r="R13" s="3" t="str">
-        <f>window_size_10!B106</f>
-        <v>Test</v>
-      </c>
-      <c r="S13" s="3" t="str">
-        <f>window_size_10!B129</f>
-        <v>Test</v>
-      </c>
-      <c r="T13" s="4" t="str">
+      <c r="B52" s="4" t="str">
         <f>window_size_5!B13</f>
         <v>Test</v>
       </c>
-      <c r="U13" s="4" t="str">
+      <c r="C52" s="4" t="str">
         <f>window_size_5!B37</f>
         <v>Test</v>
       </c>
-      <c r="V13" s="3" t="str">
+      <c r="D52" s="3" t="str">
         <f>window_size_5!B60</f>
         <v>Test</v>
       </c>
-      <c r="W13" s="3" t="str">
+      <c r="E52" s="3" t="str">
         <f>window_size_5!B83</f>
         <v>Validation</v>
       </c>
-      <c r="X13" s="3" t="str">
+      <c r="F52" s="3" t="str">
         <f>window_size_5!B106</f>
         <v>Test</v>
       </c>
-      <c r="Y13" s="3" t="str">
+      <c r="G52" s="3" t="str">
         <f>window_size_5!B129</f>
         <v>Test</v>
       </c>
@@ -4877,10 +5306,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83854168-BC43-4FD6-908E-986D692DFE20}">
-  <dimension ref="A1:B129"/>
+  <dimension ref="A1:B176"/>
   <sheetViews>
-    <sheetView topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="B117" sqref="B117:B129"/>
+    <sheetView topLeftCell="A134" workbookViewId="0">
+      <selection activeCell="B164" sqref="B164:B176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5501,6 +5930,210 @@
         <v>19</v>
       </c>
     </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B141" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B144" s="1">
+        <v>31023</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B145" s="1"/>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B146" s="1">
+        <v>0.21118012422360199</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B147" s="1">
+        <v>0.104615384615384</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B148" s="1">
+        <v>0.139917695473251</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B149" s="1">
+        <v>0.932630628888244</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B150" s="1">
+        <v>0.97839989114905701</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B151" s="1">
+        <v>0.541507637882221</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B165" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B168" s="1">
+        <v>59512</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B169" s="1"/>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B170" s="1">
+        <v>0.23651452282157601</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B171" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B172" s="1">
+        <v>0.38255033557046902</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B173" s="1">
+        <v>0.95980642559483798</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B174" s="1">
+        <v>0.95929965459154998</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B175" s="1">
+        <v>0.97964982729577499</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>